<commit_message>
Added atomic unit conversion chart
</commit_message>
<xml_diff>
--- a/unit_conversion.xlsx
+++ b/unit_conversion.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>cm-1</t>
   </si>
@@ -51,6 +52,27 @@
   </si>
   <si>
     <t>Ghz</t>
+  </si>
+  <si>
+    <t>au</t>
+  </si>
+  <si>
+    <t>nm</t>
+  </si>
+  <si>
+    <t>Ang</t>
+  </si>
+  <si>
+    <t>pm</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>km</t>
   </si>
 </sst>
 </file>
@@ -370,8 +392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,4 +718,269 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" customWidth="1"/>
+    <col min="5" max="6" width="6.7109375" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0.52917999999999998</v>
+      </c>
+      <c r="D2">
+        <f>C2*D3</f>
+        <v>5.2918E-2</v>
+      </c>
+      <c r="E2">
+        <f>C2*E3</f>
+        <v>52.917999999999999</v>
+      </c>
+      <c r="F2">
+        <f>E2*F5</f>
+        <v>5.2918000000000011E-9</v>
+      </c>
+      <c r="G2">
+        <f>F2*G6</f>
+        <v>5.2918000000000012E-11</v>
+      </c>
+      <c r="H2">
+        <f>G2*H7</f>
+        <v>5.291800000000001E-14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <f>1/C2</f>
+        <v>1.8897161646320724</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0.1</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+      <c r="F3">
+        <f>1/100000000</f>
+        <v>1E-8</v>
+      </c>
+      <c r="G3">
+        <f>F3*G6</f>
+        <v>1E-10</v>
+      </c>
+      <c r="H3">
+        <f>F3*H6</f>
+        <v>1.0000000000000002E-13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <f>1/D2</f>
+        <v>18.897161646320722</v>
+      </c>
+      <c r="C4">
+        <f>1/D3</f>
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f>E2/D2</f>
+        <v>1000</v>
+      </c>
+      <c r="F4">
+        <f>F3*C4</f>
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="G4">
+        <f>F4*G6</f>
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="H4">
+        <f>G4*H7</f>
+        <v>1.0000000000000002E-12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <f>1/E2</f>
+        <v>1.8897161646320722E-2</v>
+      </c>
+      <c r="C5">
+        <f>1/E3</f>
+        <v>0.01</v>
+      </c>
+      <c r="D5">
+        <f>1/E4</f>
+        <v>1E-3</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <f>G5*F7</f>
+        <v>1.0000000000000002E-10</v>
+      </c>
+      <c r="G5">
+        <f>G4*D5</f>
+        <v>1.0000000000000002E-12</v>
+      </c>
+      <c r="H5">
+        <f>G5*H7</f>
+        <v>1.0000000000000003E-15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <f>1/F2</f>
+        <v>188971616.46320719</v>
+      </c>
+      <c r="C6">
+        <f>1/F3</f>
+        <v>100000000</v>
+      </c>
+      <c r="D6">
+        <f>1/F4</f>
+        <v>10000000</v>
+      </c>
+      <c r="E6">
+        <f>1/F5</f>
+        <v>9999999999.9999981</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0.01</v>
+      </c>
+      <c r="H6">
+        <f>G6*H7</f>
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <f>1/G2</f>
+        <v>18897161646.320717</v>
+      </c>
+      <c r="C7">
+        <f>1/G3</f>
+        <v>10000000000</v>
+      </c>
+      <c r="D7">
+        <f>1/G4</f>
+        <v>999999999.99999988</v>
+      </c>
+      <c r="E7">
+        <f>1/G5</f>
+        <v>999999999999.99988</v>
+      </c>
+      <c r="F7">
+        <f>1/G6</f>
+        <v>100</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <f>1/H2</f>
+        <v>18897161646320.719</v>
+      </c>
+      <c r="C8">
+        <f>1/H3</f>
+        <v>9999999999999.998</v>
+      </c>
+      <c r="D8">
+        <f>1/H4</f>
+        <v>999999999999.99988</v>
+      </c>
+      <c r="E8">
+        <f>1/H5</f>
+        <v>999999999999999.75</v>
+      </c>
+      <c r="F8">
+        <f>1/H6</f>
+        <v>99999.999999999985</v>
+      </c>
+      <c r="G8">
+        <f>1/H7</f>
+        <v>1000</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>